<commit_message>
Cambios en algunas ilustraciones
Cambios en algunas ilustraciones
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion09/SolicitudGrafica_CN_10_09_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion09/SolicitudGrafica_CN_10_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\Edición Planeta\CN_10_09_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Solicitud gráfica'!$A$9:$P$92</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -556,76 +556,128 @@
     <t xml:space="preserve">Código Shutterstock 139537097. Ver obsevaciones y descripciones </t>
   </si>
   <si>
-    <t xml:space="preserve">Se solicita por favor cambiar de inglés a español los textos que aparecen en la imagen: -Solid por Sólido
+    <t>4º ESO/Fisica-quimica/ Las reacciones químicas / ¿Qué es reacción química?</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 255801601</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 94579318</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 192603359</t>
+  </si>
+  <si>
+    <t>http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=11&amp;idpil=001EQH01&amp;ruta=Buscador</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 131105219</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 252763060</t>
+  </si>
+  <si>
+    <t>Código Shutterstock 281121041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se solicita por favor realizar ilustración similar a la imagen guía. Por favor implementar imágenes que correspondan a termómetros reales </t>
+  </si>
+  <si>
+    <t>IMG02</t>
+  </si>
+  <si>
+    <t>IMG03</t>
+  </si>
+  <si>
+    <t>IMG04</t>
+  </si>
+  <si>
+    <t>IMG05</t>
+  </si>
+  <si>
+    <t>IMG06</t>
+  </si>
+  <si>
+    <t>IMG07</t>
+  </si>
+  <si>
+    <t>IMG08</t>
+  </si>
+  <si>
+    <t>IMG09</t>
+  </si>
+  <si>
+    <r>
+      <t>Se solicita por favor cambiar de inglés a español los textos que aparecen en la imagen: -Solid por Sólido
 -liquid por Líquido
 - Gas por gaseoso
 -Deposition por Sublimación
 -Sublimation por Sublimación regresiva 
 -Freezing por Solidificación 
 -Melting por Fusión
-_Evaporation por Vaporización
+_Evaporation por</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Evaporación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 -Condensation por Condensación Eliminar lo que se encuentra en el cuadro rojo 
 </t>
-  </si>
-  <si>
-    <t>Se solicita realizar ilustración de esquema igual a la imagen guía. Los colores se dejan según criterio de la diseñadora de acuerdo a maqueta.</t>
-  </si>
-  <si>
-    <t>Se solicita realizar ilustración de gráfico igual a la imagen guía. Los colores se dejan según criterio de la diseñadora de acuerdo a maqueta.</t>
-  </si>
-  <si>
-    <t>4º ESO/Fisica-quimica/ Las reacciones químicas / ¿Qué es reacción química?</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 255801601</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 94579318</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 192603359</t>
-  </si>
-  <si>
-    <t>http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=11&amp;idpil=001EQH01&amp;ruta=Buscador</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 131105219</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 252763060</t>
-  </si>
-  <si>
-    <t>Código Shutterstock 281121041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se solicita por favor realizar ilustración similar a la imagen guía. Por favor implementar imágenes que correspondan a termómetros reales </t>
-  </si>
-  <si>
-    <t>Se solicita realizar ilustración de esquema igual a la imagen guía. Los colores y formas a utilizar se dejan según criterio de la diseñadora de acuerdo a maqueta.</t>
-  </si>
-  <si>
-    <t>IMG02</t>
-  </si>
-  <si>
-    <t>IMG03</t>
-  </si>
-  <si>
-    <t>IMG04</t>
-  </si>
-  <si>
-    <t>IMG05</t>
-  </si>
-  <si>
-    <t>IMG06</t>
-  </si>
-  <si>
-    <t>IMG07</t>
-  </si>
-  <si>
-    <t>IMG08</t>
-  </si>
-  <si>
-    <t>IMG09</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se solicita realizar ilustración de gráfico igual a la imagen guía. Los colores se dejan según criterio de la diseñadora de acuerdo a maqueta. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Incluir texto Agua líquida</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se solicita realizar ilustración de esquema igual a la imagen guía. Los colores y formas a utilizar se dejan según criterio de la diseñadora de acuerdo a maqueta. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Eliminar texto vertical "Cromatografía" y Líquido gas. Adicionar Cromatografía y Decantación</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se solicita realizar ilustración de esquema igual a la imagen guía. Los colores se dejan según criterio de la diseñadora de acuerdo a maqueta. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cambiar "Vaporización" por "Evaporación"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -635,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -769,6 +821,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1761,100 +1819,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>130968</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5072061</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3333750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="Imagen 55"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="25454" t="28901" r="40184" b="27358"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14775656" y="33182719"/>
-          <a:ext cx="4941093" cy="3143250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>4438650</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>3095625</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3134" name="Object 62" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s3134"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>392906</xdr:rowOff>
@@ -1871,7 +1835,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1918,7 +1882,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1965,7 +1929,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2012,7 +1976,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2028,53 +1992,6 @@
         <a:xfrm>
           <a:off x="14942344" y="48220313"/>
           <a:ext cx="3448050" cy="2604770"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>54428</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>4819650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4374333</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Imagen 62" descr="C:\Users\Viviana\Desktop\DSC04077.JPG"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14872607" y="51230892"/>
-          <a:ext cx="4629150" cy="4319905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2106,7 +2023,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:srcRect l="27617" t="16049" r="27459" b="33187"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2149,7 +2066,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2196,7 +2113,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2243,7 +2160,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2290,7 +2207,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2337,7 +2254,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2361,6 +2278,139 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4454525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2971800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:srcRect l="38188" t="34112" r="33978" b="29664"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15354300" y="10439400"/>
+          <a:ext cx="3787775" cy="2762250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>214311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4633912</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3500436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagen 17"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15049500" y="25015030"/>
+          <a:ext cx="4229100" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>539750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3810000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3270250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagen 19"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:srcRect l="37678" t="28074" r="27698" b="25136"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15240000" y="7143750"/>
+          <a:ext cx="3238500" cy="2730500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3079,13 +3129,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3365,7 @@
     </row>
     <row r="11" spans="1:16" s="12" customFormat="1" ht="227.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>160</v>
@@ -3348,12 +3398,12 @@
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="15" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="285.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>156</v>
@@ -3386,12 +3436,12 @@
       </c>
       <c r="J12" s="67"/>
       <c r="K12" s="68" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>156</v>
@@ -3424,15 +3474,15 @@
       </c>
       <c r="J13"/>
       <c r="K13" s="68" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3465,10 +3515,10 @@
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3501,10 +3551,10 @@
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="249.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3537,10 +3587,10 @@
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="239.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3573,7 +3623,7 @@
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="348.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>156</v>
@@ -3606,7 +3656,7 @@
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="68" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3614,7 +3664,7 @@
         <v>149</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3650,7 +3700,7 @@
         <v>150</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3686,7 +3736,7 @@
         <v>151</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3722,7 +3772,7 @@
         <v>152</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3788,7 +3838,7 @@
       </c>
       <c r="J23"/>
       <c r="K23" s="68" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -5981,34 +6031,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="3134" r:id="rId4">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>4438650</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>3095625</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="3134" r:id="rId4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
 

</xml_diff>